<commit_message>
Can write actually information to a PDF, but there isn't any formatting yet
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Day</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Can now parse a csv into map rows</t>
+  </si>
+  <si>
+    <t>Can now write a basic pdf</t>
+  </si>
+  <si>
+    <t>Can no iterate through the individual sheet and print to pdf... Understand how highlighting works</t>
   </si>
 </sst>
 </file>
@@ -65,8 +71,9 @@
     <font>
       <sz val="11"/>
       <color rgb="FF444444"/>
-      <name val="Segoe UI"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -100,20 +107,23 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -398,7 +408,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -406,8 +416,8 @@
     <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" style="6" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -422,19 +432,19 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>42903</v>
+        <v>41807</v>
       </c>
       <c r="B2" s="3">
         <v>0.77083333333333337</v>
@@ -442,142 +452,163 @@
       <c r="C2" s="3">
         <v>0.77777777777777779</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="9">
         <f>HOUR(C2-B2) + MINUTE(C2-B2) / 60</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <f>SUM(D2:D100)</f>
-        <v>0.83333333333333326</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>0.81944444444444453</v>
       </c>
       <c r="C3" s="3">
         <v>0.84722222222222221</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="9">
         <f t="shared" ref="D3:D21" si="0">HOUR(C3-B3) + MINUTE(C3-B3) / 60</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.9375</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>41808</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="7">
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Printing the header and individual file results is now more modular
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Day</t>
   </si>
@@ -53,7 +53,10 @@
     <t>Can now write a basic pdf</t>
   </si>
   <si>
-    <t>Can no iterate through the individual sheet and print to pdf... Understand how highlighting works</t>
+    <t>Can now iterate through the individual sheet and print to pdf... Understand how highlighting works</t>
+  </si>
+  <si>
+    <t>Formatting the PDF</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -461,7 +464,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(D2:D100)</f>
-        <v>2.3333333333333335</v>
+        <v>4.3333333333333339</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -524,15 +527,36 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>41815</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.875</v>
+      </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>41816</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.84722222222222221</v>
+      </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Can now print team standings to a pdf
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Day</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Formatting the PDF</t>
+  </si>
+  <si>
+    <t>More formatting for the PDF generation, and now its more modular</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -464,7 +467,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(D2:D100)</f>
-        <v>4.3333333333333339</v>
+        <v>6.8333333333333339</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -558,11 +561,23 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>41827</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.875</v>
+      </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
version 0.1 found a new way to handle data management WcsfWidget screen is currently working at full capacity
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Day</t>
   </si>
@@ -60,6 +60,69 @@
   </si>
   <si>
     <t>More formatting for the PDF generation, and now its more modular</t>
+  </si>
+  <si>
+    <t>Program can now generate Team standings</t>
+  </si>
+  <si>
+    <t>Learning Kivy</t>
+  </si>
+  <si>
+    <t>Worked on file loading</t>
+  </si>
+  <si>
+    <t>Working on a useful Graphic User Interface</t>
+  </si>
+  <si>
+    <t>Continued work on the GUI</t>
+  </si>
+  <si>
+    <t>The gui can now load files and save them into a pdf</t>
+  </si>
+  <si>
+    <t>Began work on getting user input</t>
+  </si>
+  <si>
+    <t>The user can now enter division information</t>
+  </si>
+  <si>
+    <t>Organized Project folders and files</t>
+  </si>
+  <si>
+    <t>Get user input for tournament information</t>
+  </si>
+  <si>
+    <t>Get highlight color choice</t>
+  </si>
+  <si>
+    <t>You can now select trophy winners highlight color</t>
+  </si>
+  <si>
+    <t>Setting up the screen for misc player identification</t>
+  </si>
+  <si>
+    <t>Adding functionality for misc player identification</t>
+  </si>
+  <si>
+    <t>Allowed the selection of players for misc identification</t>
+  </si>
+  <si>
+    <t>Remove player identification</t>
+  </si>
+  <si>
+    <t>Saving the PDF</t>
+  </si>
+  <si>
+    <t>Severly Broke the project</t>
+  </si>
+  <si>
+    <t>Fixing the project</t>
+  </si>
+  <si>
+    <t>Failed to fix the project</t>
+  </si>
+  <si>
+    <t>Attempting to fix the way data is passed through out the application</t>
   </si>
 </sst>
 </file>
@@ -411,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -424,7 +487,7 @@
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -467,7 +530,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(D2:D100)</f>
-        <v>6.8333333333333339</v>
+        <v>29.333333333333336</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -480,7 +543,7 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:D21" si="0">HOUR(C3-B3) + MINUTE(C3-B3) / 60</f>
+        <f t="shared" ref="D3:D26" si="0">HOUR(C3-B3) + MINUTE(C3-B3) / 60</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -573,83 +636,311 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="C9" s="3">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>41829</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>41832</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>41833</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>41839</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.53125</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>41846</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>41872</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>41873</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>41876</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D22" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>41880</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D23" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>41884</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D24" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
         <v>0.875</v>
       </c>
-      <c r="D9" s="9">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="C25" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D25" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>41885</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D26" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can Highlight trophy winners now
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Day</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Finally fixed the big mistake</t>
+  </si>
+  <si>
+    <t>Finishing Touches</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -533,7 +536,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(D2:D100)</f>
-        <v>29.333333333333336</v>
+        <v>31.333333333333336</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -546,7 +549,7 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:D26" si="0">HOUR(C3-B3) + MINUTE(C3-B3) / 60</f>
+        <f t="shared" ref="D3:D27" si="0">HOUR(C3-B3) + MINUTE(C3-B3) / 60</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -947,6 +950,24 @@
       </c>
       <c r="F26" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>41886</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D27" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>